<commit_message>
luego de explicacion a Jhoan
</commit_message>
<xml_diff>
--- a/MONITOR20-2/GB/Talleres/Constantes y Variabes/revisiónConstyVar.xlsx
+++ b/MONITOR20-2/GB/Talleres/Constantes y Variabes/revisiónConstyVar.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAA7872-A207-422A-8AEE-E20476716FB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF81FAEF-A738-4460-8F7B-F4E0EB6D9478}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="reporteNotas" sheetId="1" r:id="rId1"/>
@@ -698,7 +698,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -847,6 +847,9 @@
       <c r="D11" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="3">

</xml_diff>

<commit_message>
Calificaciones Const y Var grupo B
</commit_message>
<xml_diff>
--- a/MONITOR20-2/GB/Talleres/Constantes y Variabes/revisiónConstyVar.xlsx
+++ b/MONITOR20-2/GB/Talleres/Constantes y Variabes/revisiónConstyVar.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF81FAEF-A738-4460-8F7B-F4E0EB6D9478}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DDCCBE-38BC-49A1-854F-D977E9A902F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>NO.</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>De la foto de un amigo, identifique 5 constantes y 5 variables</t>
+  </si>
+  <si>
+    <t>No presenta</t>
   </si>
 </sst>
 </file>
@@ -396,7 +399,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -698,10 +701,10 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="0.140625" customWidth="1"/>
@@ -748,6 +751,9 @@
       <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3">
@@ -775,6 +781,9 @@
       <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3">
@@ -787,6 +796,9 @@
       <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3">
@@ -799,6 +811,9 @@
       <c r="D7" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="3">
@@ -811,6 +826,9 @@
       <c r="D8" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3">
@@ -823,6 +841,9 @@
       <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="3">
@@ -835,6 +856,9 @@
       <c r="D10" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="3">
@@ -862,6 +886,9 @@
       <c r="D12" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="3">
@@ -874,6 +901,9 @@
       <c r="D13" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3">
@@ -886,6 +916,9 @@
       <c r="D14" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3">
@@ -898,6 +931,9 @@
       <c r="D15" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="3">
@@ -910,8 +946,11 @@
       <c r="D16" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -922,8 +961,11 @@
       <c r="D17" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -934,8 +976,11 @@
       <c r="D18" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -946,8 +991,11 @@
       <c r="D19" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -958,8 +1006,11 @@
       <c r="D20" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -970,8 +1021,11 @@
       <c r="D21" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -982,8 +1036,11 @@
       <c r="D22" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -994,8 +1051,11 @@
       <c r="D23" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -1006,8 +1066,11 @@
       <c r="D24" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -1018,8 +1081,11 @@
       <c r="D25" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -1030,8 +1096,11 @@
       <c r="D26" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -1042,8 +1111,14 @@
       <c r="D27" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -1053,6 +1128,9 @@
       </c>
       <c r="D28" s="5" t="s">
         <v>54</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>